<commit_message>
Deploying to gh-pages from  @ 595bfe1f0dca60ae3ccd45cbacc74ed7b0914433 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/15.4.1.xlsx
+++ b/en/downloads/data-excel/15.4.1.xlsx
@@ -128,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -160,12 +160,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -205,6 +214,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -510,11 +523,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -526,7 +537,7 @@
     <col min="6" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,7 +554,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -554,7 +565,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -585,8 +596,11 @@
       <c r="J3" s="12">
         <v>2019</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="12">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
@@ -617,8 +631,11 @@
       <c r="J4" s="14">
         <v>6.18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="14">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -628,8 +645,9 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -639,8 +657,9 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -651,7 +670,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -662,7 +681,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -673,7 +692,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>

</xml_diff>